<commit_message>
[Modify] D43020/ 43010, 43020 template/ W43010/ W43020
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/43010.xlsx
+++ b/PhoenixCI/Excel_Template/43010.xlsx
@@ -5,24 +5,27 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Bdc\結算部\風管組\個人資料區\CL.郭劻祥\1.測試\107年測試\107.1盤後子系統樣板升級\Excel_Template\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIN\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18900" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="18900" windowHeight="7944" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rpt_future" sheetId="4" r:id="rId1"/>
+    <sheet name="fut_3index" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">fut_3index!$A$1:$AG$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">rpt_future!$A$1:$N$103</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">fut_3index!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>一、</t>
   </si>
@@ -534,18 +537,546 @@
     </r>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>結算保證金</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>原始保證金</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>商品別</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>現行收取結算保證金</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>實際風險價格係數</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>適用風險價格係數</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>本日結算保證金</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動幅度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>實際風險價格係數</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>適用風險價格係數</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>本日結算保證金</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動幅度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MaxVol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>實際風險價格係數</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MaxVol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>適用風險價格係數</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MaxVol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>本日結算保證金</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動幅度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>現行</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SMA</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>EWMA</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MaxVol</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動比率</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動比率</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MaxVol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動比率</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>原保占比</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>EWMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>原保占比</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>調整後</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MaxVol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>原保占比</t>
+    </r>
+    <phoneticPr fontId="32" type="noConversion"/>
+  </si>
+  <si>
+    <t>近月份契約期貨結算價</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>契約規格</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
-    <numFmt numFmtId="177" formatCode="0.0%"/>
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="182" formatCode="#,##0_ "/>
-    <numFmt numFmtId="184" formatCode="#,##0.00_ "/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="178" formatCode="#,##0_ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="34">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -739,8 +1270,28 @@
       <family val="4"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,8 +1304,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -799,6 +1356,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -807,7 +1388,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -815,7 +1396,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="184" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -853,10 +1434,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -865,19 +1446,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -953,7 +1534,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -997,7 +1578,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1006,19 +1587,19 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -1045,6 +1626,72 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="31" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="31" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="31" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="31" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="31" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="31" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="31" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="31" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="31" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1056,6 +1703,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1443,33 +2102,33 @@
   </sheetPr>
   <dimension ref="A1:U103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" zoomScalePageLayoutView="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" zoomScalePageLayoutView="50" workbookViewId="0">
       <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="6.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="11.625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="12" customWidth="1"/>
-    <col min="6" max="6" width="11.75" style="91" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="12" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="12" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="91" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="12" customWidth="1"/>
     <col min="10" max="10" width="13" style="12" customWidth="1"/>
-    <col min="11" max="11" width="12.875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="14.125" style="45" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" style="45" customWidth="1"/>
     <col min="13" max="13" width="5" style="45" customWidth="1"/>
-    <col min="14" max="14" width="7.125" style="45" customWidth="1"/>
+    <col min="14" max="14" width="7.109375" style="45" customWidth="1"/>
     <col min="15" max="15" width="11" style="45" customWidth="1"/>
-    <col min="16" max="17" width="9.75" style="45" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.77734375" style="45" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" style="45"/>
     <col min="19" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="43.9" customHeight="1">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="43.8" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1483,11 +2142,11 @@
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="95" t="s">
+      <c r="J1" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
       <c r="M1" s="73"/>
       <c r="N1" s="74"/>
       <c r="O1" s="46"/>
@@ -1495,7 +2154,7 @@
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
     </row>
-    <row r="2" spans="1:19" s="8" customFormat="1" ht="78">
+    <row r="2" spans="1:19" s="8" customFormat="1" ht="79.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>19</v>
@@ -2114,7 +2773,7 @@
       <c r="R32" s="46"/>
       <c r="S32" s="46"/>
     </row>
-    <row r="33" spans="1:19" s="14" customFormat="1" ht="18.75">
+    <row r="33" spans="1:19" s="14" customFormat="1" ht="18">
       <c r="B33" s="70"/>
       <c r="C33" s="70"/>
       <c r="D33" s="70"/>
@@ -2133,7 +2792,7 @@
       <c r="Q33" s="51"/>
       <c r="R33" s="51"/>
     </row>
-    <row r="34" spans="1:19" s="20" customFormat="1" ht="43.9" customHeight="1">
+    <row r="34" spans="1:19" s="20" customFormat="1" ht="43.8" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
@@ -2172,7 +2831,7 @@
       <c r="K35" s="19"/>
       <c r="L35" s="54"/>
     </row>
-    <row r="36" spans="1:19" ht="57">
+    <row r="36" spans="1:19" ht="55.8">
       <c r="B36" s="7" t="s">
         <v>19</v>
       </c>
@@ -3078,7 +3737,7 @@
       <c r="L66" s="25"/>
       <c r="S66" s="45"/>
     </row>
-    <row r="67" spans="1:21" s="28" customFormat="1" ht="47.45" customHeight="1">
+    <row r="67" spans="1:21" s="28" customFormat="1" ht="47.4" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>12</v>
       </c>
@@ -3093,8 +3752,8 @@
       <c r="H67" s="12"/>
       <c r="I67" s="26"/>
       <c r="J67" s="12"/>
-      <c r="K67" s="93"/>
-      <c r="L67" s="94"/>
+      <c r="K67" s="115"/>
+      <c r="L67" s="116"/>
       <c r="M67" s="56"/>
       <c r="N67" s="56"/>
       <c r="O67" s="56"/>
@@ -3124,7 +3783,7 @@
       <c r="Q68" s="59"/>
       <c r="R68" s="59"/>
     </row>
-    <row r="69" spans="1:21" s="32" customFormat="1" ht="39">
+    <row r="69" spans="1:21" s="32" customFormat="1" ht="39.6">
       <c r="A69" s="31"/>
       <c r="B69" s="7" t="s">
         <v>19</v>
@@ -4478,7 +5137,7 @@
       <c r="T100" s="44"/>
       <c r="U100" s="44"/>
     </row>
-    <row r="101" spans="1:21" ht="23.25" customHeight="1">
+    <row r="101" spans="1:21" ht="23.4" customHeight="1">
       <c r="A101" s="2"/>
       <c r="B101" s="36" t="s">
         <v>30</v>
@@ -4504,7 +5163,7 @@
       <c r="I102" s="5"/>
       <c r="K102" s="27"/>
     </row>
-    <row r="103" spans="1:21" ht="37.15" customHeight="1">
+    <row r="103" spans="1:21" ht="37.049999999999997" customHeight="1">
       <c r="B103" s="37" t="s">
         <v>11</v>
       </c>
@@ -4531,7 +5190,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.35433070866141736" header="0.47244094488188981" footer="0"/>
-  <pageSetup paperSize="9" scale="24" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="23" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader xml:space="preserve">&amp;C&amp;"標楷體,粗體"&amp;28股票期貨契約保證金狀況表
 標的證券為受益憑證&amp;R&amp;"標楷體,標準"&amp;16
@@ -4543,4 +5202,1150 @@
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="22" style="93" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="111" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="93" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="93" customWidth="1"/>
+    <col min="5" max="16" width="10.21875" style="93" customWidth="1"/>
+    <col min="17" max="17" width="12.21875" style="109" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.109375" style="93" customWidth="1"/>
+    <col min="21" max="23" width="11.109375" style="114" customWidth="1"/>
+    <col min="24" max="24" width="11.109375" style="109" customWidth="1"/>
+    <col min="25" max="27" width="10.44140625" style="93" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" style="107" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" style="107" customWidth="1"/>
+    <col min="30" max="30" width="10.77734375" style="107" customWidth="1"/>
+    <col min="31" max="33" width="8.88671875" style="107"/>
+    <col min="34" max="16384" width="8.88671875" style="93"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="39.6" customHeight="1">
+      <c r="B1" s="93"/>
+      <c r="Q1" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="121"/>
+      <c r="Z1" s="121"/>
+      <c r="AA1" s="121"/>
+      <c r="AB1" s="121"/>
+      <c r="AC1" s="121"/>
+      <c r="AD1" s="121"/>
+      <c r="AE1" s="121"/>
+      <c r="AF1" s="121"/>
+      <c r="AG1" s="122"/>
+    </row>
+    <row r="2" spans="1:33" ht="79.2">
+      <c r="A2" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="97" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="98" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="99" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="99" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="100" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="99" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" s="112" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="112" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" s="112" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y2" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="99" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" s="101" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" s="101" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE2" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="101" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="18" customHeight="1">
+      <c r="A3" s="94"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="113"/>
+      <c r="V3" s="113"/>
+      <c r="W3" s="113"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="99"/>
+      <c r="AB3" s="113"/>
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="113"/>
+      <c r="AE3" s="106"/>
+      <c r="AF3" s="106"/>
+      <c r="AG3" s="106"/>
+    </row>
+    <row r="4" spans="1:33" ht="18" customHeight="1">
+      <c r="A4" s="94"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="113"/>
+      <c r="X4" s="99"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="99"/>
+      <c r="AB4" s="113"/>
+      <c r="AC4" s="113"/>
+      <c r="AD4" s="113"/>
+      <c r="AE4" s="106"/>
+      <c r="AF4" s="106"/>
+      <c r="AG4" s="106"/>
+    </row>
+    <row r="5" spans="1:33" ht="18" customHeight="1">
+      <c r="A5" s="94"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="97"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="99"/>
+      <c r="U5" s="113"/>
+      <c r="V5" s="113"/>
+      <c r="W5" s="113"/>
+      <c r="X5" s="99"/>
+      <c r="Y5" s="99"/>
+      <c r="Z5" s="99"/>
+      <c r="AA5" s="99"/>
+      <c r="AB5" s="113"/>
+      <c r="AC5" s="113"/>
+      <c r="AD5" s="113"/>
+      <c r="AE5" s="106"/>
+      <c r="AF5" s="106"/>
+      <c r="AG5" s="106"/>
+    </row>
+    <row r="6" spans="1:33" ht="18" customHeight="1">
+      <c r="A6" s="94"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99"/>
+      <c r="T6" s="99"/>
+      <c r="U6" s="113"/>
+      <c r="V6" s="113"/>
+      <c r="W6" s="113"/>
+      <c r="X6" s="99"/>
+      <c r="Y6" s="99"/>
+      <c r="Z6" s="99"/>
+      <c r="AA6" s="99"/>
+      <c r="AB6" s="113"/>
+      <c r="AC6" s="113"/>
+      <c r="AD6" s="113"/>
+      <c r="AE6" s="106"/>
+      <c r="AF6" s="106"/>
+      <c r="AG6" s="106"/>
+    </row>
+    <row r="7" spans="1:33" ht="18" customHeight="1">
+      <c r="A7" s="94"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="99"/>
+      <c r="T7" s="99"/>
+      <c r="U7" s="113"/>
+      <c r="V7" s="113"/>
+      <c r="W7" s="113"/>
+      <c r="X7" s="99"/>
+      <c r="Y7" s="99"/>
+      <c r="Z7" s="99"/>
+      <c r="AA7" s="99"/>
+      <c r="AB7" s="113"/>
+      <c r="AC7" s="113"/>
+      <c r="AD7" s="113"/>
+      <c r="AE7" s="106"/>
+      <c r="AF7" s="106"/>
+      <c r="AG7" s="106"/>
+    </row>
+    <row r="8" spans="1:33" ht="18" customHeight="1">
+      <c r="A8" s="94"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="102"/>
+      <c r="N8" s="102"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="99"/>
+      <c r="R8" s="99"/>
+      <c r="S8" s="99"/>
+      <c r="T8" s="99"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="99"/>
+      <c r="Y8" s="99"/>
+      <c r="Z8" s="99"/>
+      <c r="AA8" s="99"/>
+      <c r="AB8" s="113"/>
+      <c r="AC8" s="113"/>
+      <c r="AD8" s="113"/>
+      <c r="AE8" s="106"/>
+      <c r="AF8" s="106"/>
+      <c r="AG8" s="106"/>
+    </row>
+    <row r="9" spans="1:33" ht="18" customHeight="1">
+      <c r="A9" s="94"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="103"/>
+      <c r="Q9" s="99"/>
+      <c r="R9" s="99"/>
+      <c r="S9" s="99"/>
+      <c r="T9" s="99"/>
+      <c r="U9" s="113"/>
+      <c r="V9" s="113"/>
+      <c r="W9" s="113"/>
+      <c r="X9" s="99"/>
+      <c r="Y9" s="99"/>
+      <c r="Z9" s="99"/>
+      <c r="AA9" s="99"/>
+      <c r="AB9" s="113"/>
+      <c r="AC9" s="113"/>
+      <c r="AD9" s="113"/>
+      <c r="AE9" s="106"/>
+      <c r="AF9" s="106"/>
+      <c r="AG9" s="106"/>
+    </row>
+    <row r="10" spans="1:33" ht="18" customHeight="1">
+      <c r="A10" s="94"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="97"/>
+      <c r="P10" s="103"/>
+      <c r="Q10" s="99"/>
+      <c r="R10" s="99"/>
+      <c r="S10" s="99"/>
+      <c r="T10" s="99"/>
+      <c r="U10" s="113"/>
+      <c r="V10" s="113"/>
+      <c r="W10" s="113"/>
+      <c r="X10" s="99"/>
+      <c r="Y10" s="99"/>
+      <c r="Z10" s="99"/>
+      <c r="AA10" s="99"/>
+      <c r="AB10" s="113"/>
+      <c r="AC10" s="113"/>
+      <c r="AD10" s="113"/>
+      <c r="AE10" s="106"/>
+      <c r="AF10" s="106"/>
+      <c r="AG10" s="106"/>
+    </row>
+    <row r="11" spans="1:33" ht="18" customHeight="1">
+      <c r="A11" s="94"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="102"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="99"/>
+      <c r="R11" s="99"/>
+      <c r="S11" s="99"/>
+      <c r="T11" s="99"/>
+      <c r="U11" s="113"/>
+      <c r="V11" s="113"/>
+      <c r="W11" s="113"/>
+      <c r="X11" s="99"/>
+      <c r="Y11" s="99"/>
+      <c r="Z11" s="99"/>
+      <c r="AA11" s="99"/>
+      <c r="AB11" s="113"/>
+      <c r="AC11" s="113"/>
+      <c r="AD11" s="113"/>
+      <c r="AE11" s="106"/>
+      <c r="AF11" s="106"/>
+      <c r="AG11" s="106"/>
+    </row>
+    <row r="12" spans="1:33" ht="18" customHeight="1">
+      <c r="A12" s="94"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="97"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="97"/>
+      <c r="P12" s="103"/>
+      <c r="Q12" s="99"/>
+      <c r="R12" s="99"/>
+      <c r="S12" s="99"/>
+      <c r="T12" s="99"/>
+      <c r="U12" s="113"/>
+      <c r="V12" s="113"/>
+      <c r="W12" s="113"/>
+      <c r="X12" s="99"/>
+      <c r="Y12" s="99"/>
+      <c r="Z12" s="99"/>
+      <c r="AA12" s="99"/>
+      <c r="AB12" s="113"/>
+      <c r="AC12" s="113"/>
+      <c r="AD12" s="113"/>
+      <c r="AE12" s="106"/>
+      <c r="AF12" s="106"/>
+      <c r="AG12" s="106"/>
+    </row>
+    <row r="13" spans="1:33" ht="18" customHeight="1">
+      <c r="A13" s="94"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="97"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="99"/>
+      <c r="S13" s="99"/>
+      <c r="T13" s="99"/>
+      <c r="U13" s="113"/>
+      <c r="V13" s="113"/>
+      <c r="W13" s="113"/>
+      <c r="X13" s="99"/>
+      <c r="Y13" s="99"/>
+      <c r="Z13" s="99"/>
+      <c r="AA13" s="99"/>
+      <c r="AB13" s="113"/>
+      <c r="AC13" s="113"/>
+      <c r="AD13" s="113"/>
+      <c r="AE13" s="106"/>
+      <c r="AF13" s="106"/>
+      <c r="AG13" s="106"/>
+    </row>
+    <row r="14" spans="1:33" ht="18" customHeight="1">
+      <c r="A14" s="94"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="97"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="99"/>
+      <c r="R14" s="99"/>
+      <c r="S14" s="99"/>
+      <c r="T14" s="99"/>
+      <c r="U14" s="113"/>
+      <c r="V14" s="113"/>
+      <c r="W14" s="113"/>
+      <c r="X14" s="99"/>
+      <c r="Y14" s="99"/>
+      <c r="Z14" s="99"/>
+      <c r="AA14" s="99"/>
+      <c r="AB14" s="113"/>
+      <c r="AC14" s="113"/>
+      <c r="AD14" s="113"/>
+      <c r="AE14" s="106"/>
+      <c r="AF14" s="106"/>
+      <c r="AG14" s="106"/>
+    </row>
+    <row r="15" spans="1:33" ht="18" customHeight="1">
+      <c r="A15" s="94"/>
+      <c r="B15" s="110"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="97"/>
+      <c r="P15" s="103"/>
+      <c r="Q15" s="99"/>
+      <c r="R15" s="99"/>
+      <c r="S15" s="99"/>
+      <c r="T15" s="99"/>
+      <c r="U15" s="113"/>
+      <c r="V15" s="113"/>
+      <c r="W15" s="113"/>
+      <c r="X15" s="99"/>
+      <c r="Y15" s="99"/>
+      <c r="Z15" s="99"/>
+      <c r="AA15" s="99"/>
+      <c r="AB15" s="113"/>
+      <c r="AC15" s="113"/>
+      <c r="AD15" s="113"/>
+      <c r="AE15" s="106"/>
+      <c r="AF15" s="106"/>
+      <c r="AG15" s="106"/>
+    </row>
+    <row r="16" spans="1:33" ht="18" customHeight="1">
+      <c r="A16" s="94"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="97"/>
+      <c r="P16" s="103"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="99"/>
+      <c r="S16" s="99"/>
+      <c r="T16" s="99"/>
+      <c r="U16" s="113"/>
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
+      <c r="X16" s="99"/>
+      <c r="Y16" s="99"/>
+      <c r="Z16" s="99"/>
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="113"/>
+      <c r="AC16" s="113"/>
+      <c r="AD16" s="113"/>
+      <c r="AE16" s="106"/>
+      <c r="AF16" s="106"/>
+      <c r="AG16" s="106"/>
+    </row>
+    <row r="17" spans="1:33" ht="18" customHeight="1">
+      <c r="A17" s="94"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="97"/>
+      <c r="P17" s="103"/>
+      <c r="Q17" s="99"/>
+      <c r="R17" s="99"/>
+      <c r="S17" s="99"/>
+      <c r="T17" s="99"/>
+      <c r="U17" s="113"/>
+      <c r="V17" s="113"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="99"/>
+      <c r="Y17" s="99"/>
+      <c r="Z17" s="99"/>
+      <c r="AA17" s="99"/>
+      <c r="AB17" s="113"/>
+      <c r="AC17" s="113"/>
+      <c r="AD17" s="113"/>
+      <c r="AE17" s="106"/>
+      <c r="AF17" s="106"/>
+      <c r="AG17" s="106"/>
+    </row>
+    <row r="18" spans="1:33" ht="18" customHeight="1">
+      <c r="A18" s="94"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="102"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="97"/>
+      <c r="P18" s="103"/>
+      <c r="Q18" s="99"/>
+      <c r="R18" s="99"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="99"/>
+      <c r="U18" s="113"/>
+      <c r="V18" s="113"/>
+      <c r="W18" s="113"/>
+      <c r="X18" s="99"/>
+      <c r="Y18" s="99"/>
+      <c r="Z18" s="99"/>
+      <c r="AA18" s="99"/>
+      <c r="AB18" s="113"/>
+      <c r="AC18" s="113"/>
+      <c r="AD18" s="113"/>
+      <c r="AE18" s="106"/>
+      <c r="AF18" s="106"/>
+      <c r="AG18" s="106"/>
+    </row>
+    <row r="19" spans="1:33" ht="18" customHeight="1">
+      <c r="A19" s="94"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="102"/>
+      <c r="O19" s="97"/>
+      <c r="P19" s="103"/>
+      <c r="Q19" s="99"/>
+      <c r="R19" s="99"/>
+      <c r="S19" s="99"/>
+      <c r="T19" s="99"/>
+      <c r="U19" s="113"/>
+      <c r="V19" s="113"/>
+      <c r="W19" s="113"/>
+      <c r="X19" s="99"/>
+      <c r="Y19" s="99"/>
+      <c r="Z19" s="99"/>
+      <c r="AA19" s="99"/>
+      <c r="AB19" s="113"/>
+      <c r="AC19" s="113"/>
+      <c r="AD19" s="113"/>
+      <c r="AE19" s="106"/>
+      <c r="AF19" s="106"/>
+      <c r="AG19" s="106"/>
+    </row>
+    <row r="20" spans="1:33" ht="18" customHeight="1">
+      <c r="A20" s="94"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="103"/>
+      <c r="Q20" s="99"/>
+      <c r="R20" s="99"/>
+      <c r="S20" s="99"/>
+      <c r="T20" s="99"/>
+      <c r="U20" s="113"/>
+      <c r="V20" s="113"/>
+      <c r="W20" s="113"/>
+      <c r="X20" s="99"/>
+      <c r="Y20" s="99"/>
+      <c r="Z20" s="99"/>
+      <c r="AA20" s="99"/>
+      <c r="AB20" s="113"/>
+      <c r="AC20" s="113"/>
+      <c r="AD20" s="113"/>
+      <c r="AE20" s="106"/>
+      <c r="AF20" s="106"/>
+      <c r="AG20" s="106"/>
+    </row>
+    <row r="21" spans="1:33" ht="18" customHeight="1">
+      <c r="A21" s="94"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="105"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="102"/>
+      <c r="O21" s="97"/>
+      <c r="P21" s="103"/>
+      <c r="Q21" s="99"/>
+      <c r="R21" s="99"/>
+      <c r="S21" s="99"/>
+      <c r="T21" s="99"/>
+      <c r="U21" s="113"/>
+      <c r="V21" s="113"/>
+      <c r="W21" s="113"/>
+      <c r="X21" s="99"/>
+      <c r="Y21" s="99"/>
+      <c r="Z21" s="99"/>
+      <c r="AA21" s="99"/>
+      <c r="AB21" s="113"/>
+      <c r="AC21" s="113"/>
+      <c r="AD21" s="113"/>
+      <c r="AE21" s="106"/>
+      <c r="AF21" s="106"/>
+      <c r="AG21" s="106"/>
+    </row>
+    <row r="22" spans="1:33" ht="18" customHeight="1">
+      <c r="A22" s="94"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="103"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="99"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="103"/>
+      <c r="Q22" s="99"/>
+      <c r="R22" s="99"/>
+      <c r="S22" s="99"/>
+      <c r="T22" s="99"/>
+      <c r="U22" s="113"/>
+      <c r="V22" s="113"/>
+      <c r="W22" s="113"/>
+      <c r="X22" s="99"/>
+      <c r="Y22" s="99"/>
+      <c r="Z22" s="99"/>
+      <c r="AA22" s="99"/>
+      <c r="AB22" s="113"/>
+      <c r="AC22" s="113"/>
+      <c r="AD22" s="113"/>
+      <c r="AE22" s="106"/>
+      <c r="AF22" s="106"/>
+      <c r="AG22" s="106"/>
+    </row>
+    <row r="23" spans="1:33" ht="18" customHeight="1">
+      <c r="A23" s="94"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="99"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="102"/>
+      <c r="N23" s="102"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="103"/>
+      <c r="Q23" s="99"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
+      <c r="U23" s="113"/>
+      <c r="V23" s="113"/>
+      <c r="W23" s="113"/>
+      <c r="X23" s="99"/>
+      <c r="Y23" s="99"/>
+      <c r="Z23" s="99"/>
+      <c r="AA23" s="99"/>
+      <c r="AB23" s="113"/>
+      <c r="AC23" s="113"/>
+      <c r="AD23" s="113"/>
+      <c r="AE23" s="106"/>
+      <c r="AF23" s="106"/>
+      <c r="AG23" s="106"/>
+    </row>
+    <row r="24" spans="1:33" ht="18" customHeight="1">
+      <c r="A24" s="94"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="97"/>
+      <c r="P24" s="103"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="99"/>
+      <c r="S24" s="99"/>
+      <c r="T24" s="99"/>
+      <c r="U24" s="113"/>
+      <c r="V24" s="113"/>
+      <c r="W24" s="113"/>
+      <c r="X24" s="99"/>
+      <c r="Y24" s="99"/>
+      <c r="Z24" s="99"/>
+      <c r="AA24" s="99"/>
+      <c r="AB24" s="113"/>
+      <c r="AC24" s="113"/>
+      <c r="AD24" s="113"/>
+      <c r="AE24" s="106"/>
+      <c r="AF24" s="106"/>
+      <c r="AG24" s="106"/>
+    </row>
+    <row r="25" spans="1:33" ht="18" customHeight="1">
+      <c r="A25" s="94"/>
+      <c r="B25" s="110"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="97"/>
+      <c r="P25" s="103"/>
+      <c r="Q25" s="99"/>
+      <c r="R25" s="99"/>
+      <c r="S25" s="99"/>
+      <c r="T25" s="99"/>
+      <c r="U25" s="113"/>
+      <c r="V25" s="113"/>
+      <c r="W25" s="113"/>
+      <c r="X25" s="99"/>
+      <c r="Y25" s="99"/>
+      <c r="Z25" s="99"/>
+      <c r="AA25" s="99"/>
+      <c r="AB25" s="113"/>
+      <c r="AC25" s="113"/>
+      <c r="AD25" s="113"/>
+      <c r="AE25" s="106"/>
+      <c r="AF25" s="106"/>
+      <c r="AG25" s="106"/>
+    </row>
+    <row r="26" spans="1:33" ht="18" customHeight="1">
+      <c r="A26" s="94"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="99"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="102"/>
+      <c r="O26" s="97"/>
+      <c r="P26" s="103"/>
+      <c r="Q26" s="99"/>
+      <c r="R26" s="99"/>
+      <c r="S26" s="99"/>
+      <c r="T26" s="99"/>
+      <c r="U26" s="113"/>
+      <c r="V26" s="113"/>
+      <c r="W26" s="113"/>
+      <c r="X26" s="99"/>
+      <c r="Y26" s="99"/>
+      <c r="Z26" s="99"/>
+      <c r="AA26" s="99"/>
+      <c r="AB26" s="113"/>
+      <c r="AC26" s="113"/>
+      <c r="AD26" s="113"/>
+      <c r="AE26" s="106"/>
+      <c r="AF26" s="106"/>
+      <c r="AG26" s="106"/>
+    </row>
+    <row r="27" spans="1:33" ht="18" customHeight="1">
+      <c r="A27" s="94"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="102"/>
+      <c r="O27" s="97"/>
+      <c r="P27" s="103"/>
+      <c r="Q27" s="99"/>
+      <c r="R27" s="99"/>
+      <c r="S27" s="99"/>
+      <c r="T27" s="99"/>
+      <c r="U27" s="113"/>
+      <c r="V27" s="113"/>
+      <c r="W27" s="113"/>
+      <c r="X27" s="99"/>
+      <c r="Y27" s="99"/>
+      <c r="Z27" s="99"/>
+      <c r="AA27" s="99"/>
+      <c r="AB27" s="113"/>
+      <c r="AC27" s="113"/>
+      <c r="AD27" s="113"/>
+      <c r="AE27" s="106"/>
+      <c r="AF27" s="106"/>
+      <c r="AG27" s="106"/>
+    </row>
+    <row r="28" spans="1:33" ht="18" customHeight="1">
+      <c r="A28" s="94"/>
+      <c r="B28" s="110"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="99"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="102"/>
+      <c r="N28" s="102"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="103"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
+      <c r="S28" s="99"/>
+      <c r="T28" s="99"/>
+      <c r="U28" s="113"/>
+      <c r="V28" s="113"/>
+      <c r="W28" s="113"/>
+      <c r="X28" s="99"/>
+      <c r="Y28" s="99"/>
+      <c r="Z28" s="99"/>
+      <c r="AA28" s="99"/>
+      <c r="AB28" s="113"/>
+      <c r="AC28" s="113"/>
+      <c r="AD28" s="113"/>
+      <c r="AE28" s="106"/>
+      <c r="AF28" s="106"/>
+      <c r="AG28" s="106"/>
+    </row>
+    <row r="29" spans="1:33" ht="18" customHeight="1">
+      <c r="A29" s="94"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="99"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="102"/>
+      <c r="O29" s="97"/>
+      <c r="P29" s="103"/>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="99"/>
+      <c r="S29" s="99"/>
+      <c r="T29" s="99"/>
+      <c r="U29" s="113"/>
+      <c r="V29" s="113"/>
+      <c r="W29" s="113"/>
+      <c r="X29" s="99"/>
+      <c r="Y29" s="99"/>
+      <c r="Z29" s="99"/>
+      <c r="AA29" s="99"/>
+      <c r="AB29" s="113"/>
+      <c r="AC29" s="113"/>
+      <c r="AD29" s="113"/>
+      <c r="AE29" s="106"/>
+      <c r="AF29" s="106"/>
+      <c r="AG29" s="106"/>
+    </row>
+    <row r="30" spans="1:33" ht="18" customHeight="1">
+      <c r="A30" s="94"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="102"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="99"/>
+      <c r="L30" s="105"/>
+      <c r="M30" s="102"/>
+      <c r="N30" s="102"/>
+      <c r="O30" s="97"/>
+      <c r="P30" s="103"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99"/>
+      <c r="T30" s="99"/>
+      <c r="U30" s="113"/>
+      <c r="V30" s="113"/>
+      <c r="W30" s="113"/>
+      <c r="X30" s="99"/>
+      <c r="Y30" s="99"/>
+      <c r="Z30" s="99"/>
+      <c r="AA30" s="99"/>
+      <c r="AB30" s="113"/>
+      <c r="AC30" s="113"/>
+      <c r="AD30" s="113"/>
+      <c r="AE30" s="106"/>
+      <c r="AF30" s="106"/>
+      <c r="AG30" s="106"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="X1:AG1"/>
+  </mergeCells>
+  <phoneticPr fontId="32" type="noConversion"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="16" max="29" man="1"/>
+  </colBreaks>
+</worksheet>
 </file>
</xml_diff>